<commit_message>
Doc reference and clause mapping with docx extract
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G94"/>
+  <dimension ref="A1:I94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,30 +436,40 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Clause</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Section</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Control Id</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Control Title</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Compliance</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Reference</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Gaps Identified</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Recommended Action</t>
         </is>
@@ -471,32 +481,42 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>4,5</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>A.5.1</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>Policies for information security</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>🟡</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>The document includes a Business Continuity Plan and references an IT Security Policy but does not explicitly present or reference a comprehensive information security policy covering all aspects required by ISO/IEC 27001:2022 A.5.1.</t>
-        </is>
-      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Develop and formally document a comprehensive Information Security Policy that addresses all relevant aspects of information security and ensure it is approved and communicated to all relevant stakeholders.</t>
+          <t>The document includes a Business Continuity Plan and references an IT Security Policy but does not explicitly present a comprehensive information security policy covering all aspects required by ISO/IEC 27001.</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Lack of a clearly defined, organization-wide information security policy document within the provided text.</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Develop and formally document a comprehensive information security policy aligned with ISO/IEC 27001 requirements and ensure it is communicated to all relevant stakeholders.</t>
         </is>
       </c>
     </row>
@@ -506,26 +526,36 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>4,5</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>A.5.2</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>Information security roles and responsibilities</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>✅</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Section 2.3 Appointments and authorities (Pages 4-6) clearly defines roles such as Crisis Management Team, Crisis Management Support Team, Operational Director, Recovery Managers, and their responsibilities during disruptive incidents.</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -533,32 +563,42 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>A.5.3</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>Segregation of duties</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>No evidence of segregation of duties controls or policies to reduce risk of unauthorized or unintentional modification or misuse of information or assets.</t>
+          <t>🟡</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Define and implement segregation of duties policies and procedures to ensure critical tasks are divided among different individuals to reduce risk.</t>
+          <t>The document defines roles and responsibilities but does not explicitly address segregation of duties to prevent conflicts of interest or fraud.</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>No explicit mention or evidence of segregation of duties controls.</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Implement and document segregation of duties policies to ensure critical tasks are divided among different individuals to reduce risk.</t>
         </is>
       </c>
     </row>
@@ -568,86 +608,108 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>5,6,9,10</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>A.5.4</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>Management responsibilities</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>✅</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Management responsibilities are detailed in Sections 2.3, 3.2, and 3.3, including decision-making authority, resource allocation, communication, and review processes.</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
         <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>A.5.5</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>Contact with authorities</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>✅</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Appendix 1 Incident Response Plan (Page 11) includes contacts with local authorities (police, fire department, call 112) for facility disasters and incidents.</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
         <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>A.5.6</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>Contact with special interest groups</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>No mention of contact or engagement with special interest groups or professional bodies related to information security.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Establish and document procedures for maintaining contact with relevant special interest groups and professional bodies to stay informed on security trends and threats.</t>
+          <t>No mention of contact with special interest groups or participation in information security forums or groups.</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Lack of documented contact or engagement with special interest groups related to information security.</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Establish and document procedures for maintaining contact with relevant special interest groups to stay informed on security trends and threats.</t>
         </is>
       </c>
     </row>
@@ -657,32 +719,42 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>A.5.7</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>Threat intelligence</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>No evidence of processes or mechanisms for gathering, analyzing, and using threat intelligence.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Implement a threat intelligence process to collect and analyze relevant threat information to support risk management and incident response.</t>
+          <t>No evidence of processes or procedures for gathering, analyzing, or using threat intelligence.</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Absence of documented threat intelligence activities.</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Implement a threat intelligence process to collect and analyze relevant security threat information and integrate it into risk management.</t>
         </is>
       </c>
     </row>
@@ -692,32 +764,42 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>A.5.8</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>Information security in project management</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>No reference to integrating information security requirements into project management processes.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Incorporate information security requirements and controls into project management methodologies and document this integration.</t>
+          <t>No reference to integrating information security requirements into project management activities.</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Lack of documented controls or processes addressing information security in project management.</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Incorporate information security requirements and controls into project management methodologies and document accordingly.</t>
         </is>
       </c>
     </row>
@@ -725,34 +807,40 @@
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
         <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>A.5.9</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>Inventory of information and other associated assets</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>🟡</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>The document references lists of business continuity sites and recovery plans but does not explicitly provide or reference a comprehensive inventory of information and associated assets.</t>
-        </is>
-      </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Develop and maintain a detailed inventory of information assets and associated assets, including ownership and classification.</t>
+          <t>Section 3.1 mentions evaluation of damaged assets including name, location, type, and cost, but no comprehensive inventory of all information assets is presented.</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>No formal, comprehensive inventory of information and associated assets documented.</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Develop and maintain a formal inventory of all information assets and associated assets as part of the ISMS.</t>
         </is>
       </c>
     </row>
@@ -762,32 +850,42 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>A.5.10</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>Acceptable use of information and other associated assets</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>No policies or rules regarding acceptable use of information and assets are documented.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Establish and communicate an Acceptable Use Policy covering information and associated assets.</t>
+          <t>No policies or rules regarding acceptable use of information or assets are included in the document.</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Absence of acceptable use policies for information and assets.</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Develop and communicate acceptable use policies covering information and associated assets.</t>
         </is>
       </c>
     </row>
@@ -795,34 +893,40 @@
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
         <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>A.5.11</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>Return of assets</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>No procedures or policies addressing the return of assets upon termination or change of employment or contract.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Define and implement procedures to ensure return of organizational assets when no longer required or upon termination.</t>
+          <t>No mention of procedures for return of assets upon termination or role change.</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Lack of documented procedures for return of assets.</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Establish and document procedures to ensure return of organizational assets when no longer required or upon termination.</t>
         </is>
       </c>
     </row>
@@ -832,32 +936,42 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>A.5.12</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>Classification of information</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>No evidence of information classification scheme or policies.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Develop and implement an information classification policy and scheme to categorize information based on sensitivity and impact.</t>
+          <t>No evidence of information classification scheme or process.</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>No documented information classification policy or scheme.</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Develop and implement an information classification scheme and associated policies.</t>
         </is>
       </c>
     </row>
@@ -865,32 +979,38 @@
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
         <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>A.5.13</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>Labelling of information</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F14" t="inlineStr">
         <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
           <t>No mention of labelling requirements or procedures for classified information.</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>No documented labelling procedures for information.</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
         <is>
           <t>Establish labelling procedures aligned with the information classification scheme.</t>
         </is>
@@ -902,32 +1022,42 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>4,8</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>A.5.14</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>Information transfer</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>No documented controls or procedures for secure information transfer.</t>
+          <t>🟡</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Implement and document secure information transfer policies and procedures.</t>
+          <t>Communication methods and responsibilities are described (Section 2.5), but no explicit controls or policies for secure information transfer are documented.</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Lack of documented secure information transfer policies and controls.</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Develop and implement policies and procedures to ensure secure transfer of information internally and externally.</t>
         </is>
       </c>
     </row>
@@ -935,34 +1065,40 @@
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
         <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>A.5.15</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>Access control</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>No explicit access control policies or procedures described.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Develop and enforce access control policies and procedures to restrict access to information and assets.</t>
+          <t>No specific access control policies or procedures are described in the document.</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Absence of documented access control measures.</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Establish and document access control policies and procedures aligned with ISO/IEC 27001.</t>
         </is>
       </c>
     </row>
@@ -970,34 +1106,40 @@
       <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr">
         <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>A.5.16</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>Identity management</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F17" t="inlineStr">
         <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
           <t>No mention of identity management processes or controls.</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>Implement identity management processes to ensure proper identification and management of users.</t>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Lack of documented identity management controls.</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Implement and document identity management processes to ensure proper identification and authentication of users.</t>
         </is>
       </c>
     </row>
@@ -1005,34 +1147,40 @@
       <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr">
         <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>A.5.17</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>Authentication information</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>No documented controls or policies for managing authentication information.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Establish policies and procedures for secure management of authentication information.</t>
+          <t>No details on management of authentication information such as passwords or tokens.</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>No documented controls for authentication information management.</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Develop policies and procedures for secure management of authentication information.</t>
         </is>
       </c>
     </row>
@@ -1040,34 +1188,40 @@
       <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr">
         <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>A.5.18</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>Access rights</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>No evidence of formal processes for granting, reviewing, and revoking access rights.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Define and implement access rights management processes including periodic review.</t>
+          <t>No documented process for granting, reviewing, or revoking access rights.</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Absence of access rights management procedures.</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Establish and maintain formal procedures for access rights management.</t>
         </is>
       </c>
     </row>
@@ -1077,30 +1231,40 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
+          <t>4,8</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>A.5.19</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>Information security in supplier relationships</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>🟡</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>The document references contacts with vendors and suppliers but lacks documented information security requirements or controls in supplier relationships.</t>
-        </is>
-      </c>
       <c r="G20" t="inlineStr">
+        <is>
+          <t>Supplier contacts and responsibilities are listed (Appendix 5), but no formal information security requirements or controls for supplier relationships are documented.</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Lack of documented information security controls in supplier relationships.</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
         <is>
           <t>Develop and implement information security requirements and controls for managing supplier relationships.</t>
         </is>
@@ -1112,32 +1276,42 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>A.5.20</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>Addressing information security within supplier agreements</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="F21" t="inlineStr">
         <is>
           <t>🟡</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Supplier agreements are referenced indirectly via vendor contacts and incident response contacts, but there is no explicit mention of addressing information security requirements within supplier agreements.</t>
-        </is>
-      </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Include explicit clauses or policies that define information security requirements to be included in supplier agreements and ensure these are documented and managed.</t>
+          <t>Section 2.8 mentions dependencies and interactions with suppliers and external parties detailed in Incident Response Plan, Disaster Recovery Plan, and recovery plans, but no explicit mention of addressing information security requirements within supplier agreements.</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Lack of explicit clauses or controls addressing information security requirements within supplier agreements.</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Include explicit requirements and clauses in supplier agreements to address information security obligations and responsibilities.</t>
         </is>
       </c>
     </row>
@@ -1147,32 +1321,42 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>A.5.21</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>Managing information security in the ICT supply chain</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>🟡</t>
-        </is>
-      </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>The document references suppliers and external parties in recovery plans and incident response, but lacks a formal process or controls specifically for managing information security risks in the ICT supply chain.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Develop and document processes to assess and manage information security risks related to ICT suppliers and the supply chain.</t>
+          <t>No explicit mention or description of managing information security risks in the ICT supply chain found in the document.</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>No documented processes or controls for managing information security risks in the ICT supply chain.</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Develop and document controls and processes to manage information security risks in the ICT supply chain.</t>
         </is>
       </c>
     </row>
@@ -1182,32 +1366,42 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>A.5.22</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>Monitoring, review and change management of supplier services</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>No mention of monitoring, reviewing, or managing changes in supplier services is found in the document.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Establish and document procedures for ongoing monitoring, review, and change management of supplier services to ensure continued compliance with information security requirements.</t>
+          <t>No references found regarding monitoring, review, or change management of supplier services.</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Absence of documented procedures for monitoring and reviewing supplier services or managing changes.</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Establish and document procedures for ongoing monitoring, review, and change management of supplier services.</t>
         </is>
       </c>
     </row>
@@ -1217,32 +1411,42 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>A.5.23</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>Information security for use of cloud services</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="F24" t="inlineStr">
         <is>
           <t>🟡</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Cloud services are mentioned (e.g., CRM Cloud system, cloud-based telephony, Google Drive storage), but there is no explicit information security control or policy addressing cloud service usage.</t>
-        </is>
-      </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Define and document information security requirements and controls specific to the use of cloud services, including risk assessments and supplier security obligations.</t>
+          <t>Cloud services such as CRM Cloud system and cloud-based telephony (3CX) are mentioned with recovery times and responsible persons, but no explicit information security controls or policies for cloud services are detailed.</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Lack of explicit information security controls or policies specific to cloud service usage.</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Define and document information security requirements and controls specific to cloud services usage.</t>
         </is>
       </c>
     </row>
@@ -1252,26 +1456,36 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>A.5.24</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>Information security incident management planning and preparation</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="F25" t="inlineStr">
         <is>
           <t>✅</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Appendix 1 Incident Response Plan, Section 2.4 Plan activation/deactivation, and detailed incident response procedures demonstrate planning and preparation for information security incidents.</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1279,26 +1493,36 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
+          <t>8,10</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>A.5.25</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="E26" t="inlineStr">
         <is>
           <t>Assessment and decision on information security events</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="F26" t="inlineStr">
         <is>
           <t>✅</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Section 3.2 describes assessment of the situation and decision-making by the Operational Director regarding incident response and recovery actions.</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1306,26 +1530,36 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>8,10</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>A.5.26</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>Response to information security incidents</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="F27" t="inlineStr">
         <is>
           <t>✅</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Appendix 1 Incident Response Plan and Section 2.4 describe activation and response procedures for incidents.</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1333,32 +1567,42 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
+          <t>8,10</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>A.5.27</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="E28" t="inlineStr">
         <is>
           <t>Learning from information security incidents</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="F28" t="inlineStr">
         <is>
           <t>🟡</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>The document includes incident logging and response but does not explicitly describe processes for learning from incidents or implementing improvements based on lessons learned.</t>
-        </is>
-      </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Implement and document a formal process for post-incident review and continuous improvement based on lessons learned from information security incidents.</t>
+          <t>Section 4 mentions evaluation criteria including whether recovery plans and incident response plans are synchronized and if exercising/testing achieved objectives, implying some review, but no explicit process for learning from incidents.</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>No explicit documented process for post-incident review and learning.</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Implement and document a formal process for post-incident review and incorporation of lessons learned.</t>
         </is>
       </c>
     </row>
@@ -1368,32 +1612,42 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>A.5.28</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t>Collection of evidence</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>🟡</t>
-        </is>
-      </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Preservation of damaged assets is mentioned, but there is no detailed procedure for collection, handling, and preservation of digital or physical evidence related to information security incidents.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Develop and document procedures for evidence collection, handling, and preservation to support investigations and potential legal actions.</t>
+          <t>No mention of procedures or controls for collection, preservation, or handling of evidence related to information security incidents.</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Absence of documented evidence collection procedures.</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Develop and document procedures for proper collection and handling of evidence during information security incidents.</t>
         </is>
       </c>
     </row>
@@ -1401,55 +1655,67 @@
       <c r="A30" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr">
         <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>A.5.29</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="E30" t="inlineStr">
         <is>
           <t>Information security during disruption</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
+      <c r="F30" t="inlineStr">
         <is>
           <t>✅</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>The entire Business Continuity Plan focuses on managing information security and business continuity during disruptions, including recovery plans and communication.</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr">
         <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="D31" t="inlineStr">
         <is>
           <t>A.5.30</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="E31" t="inlineStr">
         <is>
           <t>ICT readiness for business continuity</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="F31" t="inlineStr">
         <is>
           <t>✅</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Section 2.9 Required resources and Disaster Recovery Plans demonstrate ICT readiness for business continuity.</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1457,26 +1723,36 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>A.5.31</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="E32" t="inlineStr">
         <is>
           <t>Identification of legal, statutory, regulatory and contractual requirements</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
+      <c r="F32" t="inlineStr">
         <is>
           <t>✅</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Chapter 1 Reference documents includes 'List of Legal, Regulatory, Contractual and Other Requirements'.</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1484,32 +1760,42 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="D33" t="inlineStr">
         <is>
           <t>A.5.32</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="E33" t="inlineStr">
         <is>
           <t>Intellectual property rights</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>No reference to intellectual property rights protection or management is found in the document.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Include policies and controls addressing the protection and management of intellectual property rights.</t>
+          <t>No mention of intellectual property rights protection or related controls.</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>No documented controls or policies addressing intellectual property rights.</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Include policies and controls to protect intellectual property rights.</t>
         </is>
       </c>
     </row>
@@ -1519,32 +1805,42 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="D34" t="inlineStr">
         <is>
           <t>A.5.33</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="E34" t="inlineStr">
         <is>
           <t>Protection of records</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="F34" t="inlineStr">
         <is>
           <t>🟡</t>
         </is>
       </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>The document mentions storage locations for the Business Continuity Plan but lacks detailed controls for protection, retention, and integrity of records.</t>
-        </is>
-      </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Define and implement controls for protection, retention, and integrity of records relevant to information security and business continuity.</t>
+          <t>Chapter 4 Validity and document management describes storage of paper and electronic documents but lacks detailed controls on protection of records.</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Insufficient detail on protection measures for records (e.g., access control, retention).</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>Enhance documentation with specific controls for protection, retention, and access to records.</t>
         </is>
       </c>
     </row>
@@ -1554,32 +1850,42 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="D35" t="inlineStr">
         <is>
           <t>A.5.34</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="E35" t="inlineStr">
         <is>
           <t>Privacy and protection of PII</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
+      <c r="F35" t="inlineStr">
         <is>
           <t>🟡</t>
         </is>
       </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>Data leakage (GDPR) is mentioned in incident response, but there is no comprehensive privacy policy or controls for protection of personally identifiable information (PII).</t>
-        </is>
-      </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Develop and document privacy policies and controls to protect PII in compliance with applicable regulations such as GDPR.</t>
+          <t>Incident Response Plan includes data leakage (GDPR) incident handling and contact with authorities, but no comprehensive privacy policy or controls detailed.</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Lack of comprehensive privacy and PII protection policies and controls.</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Develop and document comprehensive privacy policies and controls for PII protection.</t>
         </is>
       </c>
     </row>
@@ -1589,32 +1895,42 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
+          <t>5,9</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="D36" t="inlineStr">
         <is>
           <t>A.5.35</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="E36" t="inlineStr">
         <is>
           <t>Independent review of information security</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>No mention of independent or external reviews or audits of information security is found.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Establish and document a process for independent review or audit of the information security management system and related controls.</t>
+          <t>No mention of independent reviews or audits of information security.</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>No documented independent review or audit processes.</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>Establish and document independent review or audit processes for information security.</t>
         </is>
       </c>
     </row>
@@ -1624,32 +1940,42 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
+          <t>5,9,10</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="D37" t="inlineStr">
         <is>
           <t>A.5.36</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="E37" t="inlineStr">
         <is>
           <t>Compliance with policies and standards for information security</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
+      <c r="F37" t="inlineStr">
         <is>
           <t>🟡</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>The document references ISO standards and policies but does not explicitly describe how compliance with information security policies and standards is monitored or enforced.</t>
-        </is>
-      </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Implement and document processes to monitor and ensure compliance with information security policies and standards.</t>
+          <t>Document mentions evaluation criteria and responsibilities but lacks explicit compliance monitoring or enforcement mechanisms.</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>No explicit compliance monitoring or enforcement processes described.</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>Implement and document compliance monitoring and enforcement mechanisms.</t>
         </is>
       </c>
     </row>
@@ -1657,28 +1983,42 @@
       <c r="A38" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="B38" t="inlineStr"/>
+      <c r="C38" t="inlineStr">
         <is>
           <t>A.5 (Organisational Controls)</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="D38" t="inlineStr">
         <is>
           <t>A.5.37</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="E38" t="inlineStr">
         <is>
           <t>Documented operating procedures</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>✅</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr"/>
-      <c r="G38" t="inlineStr"/>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>🟡</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Some documented plans and procedures exist (e.g., Incident Response Plan, Disaster Recovery Plan), but no comprehensive documented operating procedures for all relevant processes.</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Incomplete documented operating procedures for all ISMS processes.</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Develop and maintain comprehensive documented operating procedures.</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1686,32 +2026,42 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
           <t>A.6 (People Controls)</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="D39" t="inlineStr">
         <is>
           <t>A.6.1</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
+      <c r="E39" t="inlineStr">
         <is>
           <t>Screening</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>No information on personnel screening or background checks is provided in the document.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Develop and implement personnel screening procedures as part of the human resource security controls.</t>
+          <t>No mention of personnel screening or background checks.</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>No documented personnel screening processes.</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Implement and document personnel screening procedures.</t>
         </is>
       </c>
     </row>
@@ -1721,32 +2071,42 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
           <t>A.6 (People Controls)</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="D40" t="inlineStr">
         <is>
           <t>A.6.2</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="E40" t="inlineStr">
         <is>
           <t>Terms and conditions of employment</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>The document does not mention terms and conditions of employment or how information security requirements are integrated into employment contracts.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Include policies or procedures that define and communicate information security terms and conditions in employment contracts.</t>
+          <t>No mention of terms and conditions of employment in the document.</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>The document does not address terms and conditions of employment related to information security.</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Include policies or references to terms and conditions of employment that specify information security responsibilities and expectations.</t>
         </is>
       </c>
     </row>
@@ -1756,30 +2116,40 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
           <t>A.6 (People Controls)</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="D41" t="inlineStr">
         <is>
           <t>A.6.3</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="E41" t="inlineStr">
         <is>
           <t>Information security awareness, education and training</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>No reference to information security awareness, education, or training programs for employees is found in the document.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
+        <is>
+          <t>No information security awareness, education or training programs mentioned.</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Lack of documented information security awareness, education, and training for personnel.</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
         <is>
           <t>Develop and document an information security awareness, education, and training program for all employees.</t>
         </is>
@@ -1791,32 +2161,42 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
           <t>A.6 (People Controls)</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="D42" t="inlineStr">
         <is>
           <t>A.6.4</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
+      <c r="E42" t="inlineStr">
         <is>
           <t>Disciplinary process</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>The document does not address disciplinary processes related to information security breaches or violations.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Establish and document a disciplinary process for information security violations.</t>
+          <t>No disciplinary process related to information security is described.</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>No disciplinary process for information security breaches or violations is documented.</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>Establish and document a disciplinary process for handling information security violations.</t>
         </is>
       </c>
     </row>
@@ -1826,32 +2206,42 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
           <t>A.6 (People Controls)</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="D43" t="inlineStr">
         <is>
           <t>A.6.5</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="E43" t="inlineStr">
         <is>
           <t>Responsibilities after termination or change of employment</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>No mention of responsibilities or controls related to employees after termination or change of employment.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Define and document responsibilities and controls for employees after termination or change of employment, including return of assets and revocation of access.</t>
+          <t>No mention of responsibilities after termination or change of employment.</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>No procedures or responsibilities defined for employees after termination or change of employment.</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>Define and document responsibilities and actions to be taken after termination or change of employment to protect information security.</t>
         </is>
       </c>
     </row>
@@ -1859,34 +2249,40 @@
       <c r="A44" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="B44" t="inlineStr"/>
+      <c r="C44" t="inlineStr">
         <is>
           <t>A.6 (People Controls)</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="D44" t="inlineStr">
         <is>
           <t>A.6.6</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="E44" t="inlineStr">
         <is>
           <t>Confidentiality or non-disclosure agreements</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>The document does not mention confidentiality or non-disclosure agreements for employees or contractors.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Implement and document confidentiality or non-disclosure agreements as part of employment or contractor onboarding.</t>
+          <t>No mention of confidentiality or non-disclosure agreements in the document.</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>No evidence of confidentiality or non-disclosure agreements for personnel.</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>Implement and document confidentiality or non-disclosure agreements for all relevant personnel.</t>
         </is>
       </c>
     </row>
@@ -1894,34 +2290,40 @@
       <c r="A45" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="inlineStr">
         <is>
           <t>A.6 (People Controls)</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="D45" t="inlineStr">
         <is>
           <t>A.6.7</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
+      <c r="E45" t="inlineStr">
         <is>
           <t>Remote working</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr">
+      <c r="F45" t="inlineStr">
         <is>
           <t>🟡</t>
         </is>
       </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>The document states that all employees except the Studio Department can work from home in the cloud, but lacks detailed security controls or policies for remote working.</t>
-        </is>
-      </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Develop and document comprehensive remote working policies including security requirements, access controls, and monitoring.</t>
+          <t>Section 2.6 and 2.9 mention employees working from home in the cloud and transportation plans.</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Remote working is acknowledged but lacks detailed information security controls or policies specific to remote work.</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>Develop and document specific information security policies and controls for remote working.</t>
         </is>
       </c>
     </row>
@@ -1929,28 +2331,42 @@
       <c r="A46" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="B46" t="inlineStr">
+      <c r="B46" t="inlineStr"/>
+      <c r="C46" t="inlineStr">
         <is>
           <t>A.6 (People Controls)</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="D46" t="inlineStr">
         <is>
           <t>A.6.8</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
+      <c r="E46" t="inlineStr">
         <is>
           <t>Information security event reporting</t>
         </is>
       </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>✅</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr"/>
-      <c r="G46" t="inlineStr"/>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>🟡</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Appendix 1 Incident Response Plan and Appendix 2 Incident Log describe incident reporting procedures for IT and facilities incidents.</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Event reporting is addressed but could be more comprehensive and explicitly linked to all types of information security events.</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>Enhance and formalize the information security event reporting process to cover all relevant events and ensure timely reporting.</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -1958,32 +2374,42 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
           <t>A.7 (Physical Controls)</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="D47" t="inlineStr">
         <is>
           <t>A.7.1</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
+      <c r="E47" t="inlineStr">
         <is>
           <t>Physical security perimeter</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>No description of physical security perimeters or boundaries protecting facilities is provided.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Define and document physical security perimeters for all facilities.</t>
+          <t>No description of physical security perimeters or controls around facilities.</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Physical security perimeter controls are not documented.</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>Define and document physical security perimeter controls to protect facilities.</t>
         </is>
       </c>
     </row>
@@ -1991,34 +2417,40 @@
       <c r="A48" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="B48" t="inlineStr"/>
+      <c r="C48" t="inlineStr">
         <is>
           <t>A.7 (Physical Controls)</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="D48" t="inlineStr">
         <is>
           <t>A.7.2</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
+      <c r="E48" t="inlineStr">
         <is>
           <t>Physical entry controls</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>No information on physical entry controls such as access cards, locks, or visitor management.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Implement and document physical entry control measures.</t>
+          <t>No mention of physical entry controls or access restrictions.</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>No physical entry control measures are described.</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>Implement and document physical entry controls to restrict access to secure areas.</t>
         </is>
       </c>
     </row>
@@ -2026,32 +2458,38 @@
       <c r="A49" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="B49" t="inlineStr"/>
+      <c r="C49" t="inlineStr">
         <is>
           <t>A.7 (Physical Controls)</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="D49" t="inlineStr">
         <is>
           <t>A.7.3</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="E49" t="inlineStr">
         <is>
           <t>Securing offices, rooms and facilities</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>No details on securing offices, rooms, or facilities against unauthorized access or environmental threats.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
+        <is>
+          <t>No information on securing offices, rooms, or facilities.</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>No documented controls for securing physical locations.</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
         <is>
           <t>Establish and document procedures for securing offices, rooms, and facilities.</t>
         </is>
@@ -2063,32 +2501,42 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
           <t>A.7 (Physical Controls)</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="D50" t="inlineStr">
         <is>
           <t>A.7.4</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
+      <c r="E50" t="inlineStr">
         <is>
           <t>Physical security monitoring</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>No mention of physical security monitoring such as CCTV or alarm systems.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Implement physical security monitoring controls and document their use.</t>
+          <t>No mention of physical security monitoring such as CCTV or alarms.</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Physical security monitoring controls are missing.</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>Implement physical security monitoring measures and document them.</t>
         </is>
       </c>
     </row>
@@ -2096,34 +2544,40 @@
       <c r="A51" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="B51" t="inlineStr"/>
+      <c r="C51" t="inlineStr">
         <is>
           <t>A.7 (Physical Controls)</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="D51" t="inlineStr">
         <is>
           <t>A.7.5</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
+      <c r="E51" t="inlineStr">
         <is>
           <t>Protecting against physical and environmental threats</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>No controls or procedures addressing protection against physical and environmental threats are described.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Develop and document measures to protect facilities and assets from physical and environmental threats.</t>
+          <t>No controls addressing physical or environmental threats are described.</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>No documented protection against physical and environmental threats.</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>Develop and document controls to protect against physical and environmental threats.</t>
         </is>
       </c>
     </row>
@@ -2131,34 +2585,40 @@
       <c r="A52" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="B52" t="inlineStr">
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="inlineStr">
         <is>
           <t>A.7 (Physical Controls)</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
+      <c r="D52" t="inlineStr">
         <is>
           <t>A.7.6</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr">
+      <c r="E52" t="inlineStr">
         <is>
           <t>Working in secure areas</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>No information on controls for working in secure areas or restricted zones.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Define and implement controls for working in secure areas.</t>
+          <t>No mention of controls for working in secure areas.</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>No procedures or controls for working in secure areas.</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>Define and document controls for working in secure areas.</t>
         </is>
       </c>
     </row>
@@ -2166,34 +2626,40 @@
       <c r="A53" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="B53" t="inlineStr">
+      <c r="B53" t="inlineStr"/>
+      <c r="C53" t="inlineStr">
         <is>
           <t>A.7 (Physical Controls)</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
+      <c r="D53" t="inlineStr">
         <is>
           <t>A.7.7</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
+      <c r="E53" t="inlineStr">
         <is>
           <t>Clear desk and clear screen</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>No mention of clear desk and clear screen policies to protect sensitive information.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Establish and communicate clear desk and clear screen policies.</t>
+          <t>No mention of clear desk or clear screen policies.</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>No clear desk and clear screen policies documented.</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>Implement and communicate clear desk and clear screen policies.</t>
         </is>
       </c>
     </row>
@@ -2201,34 +2667,40 @@
       <c r="A54" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="B54" t="inlineStr">
+      <c r="B54" t="inlineStr"/>
+      <c r="C54" t="inlineStr">
         <is>
           <t>A.7 (Physical Controls)</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
+      <c r="D54" t="inlineStr">
         <is>
           <t>A.7.8</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr">
+      <c r="E54" t="inlineStr">
         <is>
           <t>Equipment siting and protection</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>No details on equipment siting and protection to reduce risks of theft or damage.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Document procedures for equipment siting and protection.</t>
+          <t>No information on equipment siting and protection.</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>No documented controls for equipment siting and protection.</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>Establish and document controls for equipment siting and protection.</t>
         </is>
       </c>
     </row>
@@ -2236,34 +2708,40 @@
       <c r="A55" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="B55" t="inlineStr">
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="inlineStr">
         <is>
           <t>A.7 (Physical Controls)</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
+      <c r="D55" t="inlineStr">
         <is>
           <t>A.7.9</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr">
+      <c r="E55" t="inlineStr">
         <is>
           <t>Security of assets off-premises</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>No controls or guidance on security of assets taken off-premises.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Implement policies and controls for securing assets off-premises.</t>
+          <t>No mention of security controls for assets off-premises.</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>No controls for security of assets off-premises.</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>Define and document security controls for assets used or stored off-premises.</t>
         </is>
       </c>
     </row>
@@ -2271,34 +2749,40 @@
       <c r="A56" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="B56" t="inlineStr">
+      <c r="B56" t="inlineStr"/>
+      <c r="C56" t="inlineStr">
         <is>
           <t>A.7 (Physical Controls)</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
+      <c r="D56" t="inlineStr">
         <is>
           <t>A.7.10</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
+      <c r="E56" t="inlineStr">
         <is>
           <t>Storage media</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>No mention of controls for secure handling, storage, and disposal of storage media.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Define and document controls for storage media management.</t>
+          <t>No mention of controls for storage media.</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>No documented controls for handling and protecting storage media.</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>Implement and document controls for storage media protection and handling.</t>
         </is>
       </c>
     </row>
@@ -2306,34 +2790,40 @@
       <c r="A57" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="B57" t="inlineStr">
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="inlineStr">
         <is>
           <t>A.7 (Physical Controls)</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
+      <c r="D57" t="inlineStr">
         <is>
           <t>A.7.11</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
+      <c r="E57" t="inlineStr">
         <is>
           <t>Supporting utilities</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr">
+      <c r="F57" t="inlineStr">
         <is>
           <t>🟡</t>
         </is>
       </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>The document lists utilities such as electricity and internet access with responsible persons, but lacks detailed controls to ensure their security and availability.</t>
-        </is>
-      </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Develop and document controls to secure supporting utilities and ensure their availability.</t>
+          <t>Section 2.9 lists electricity and internet access as external services with responsible persons.</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>Supporting utilities are identified but no detailed controls or risk management described.</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>Develop detailed controls and contingency plans for supporting utilities.</t>
         </is>
       </c>
     </row>
@@ -2341,34 +2831,40 @@
       <c r="A58" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="B58" t="inlineStr">
+      <c r="B58" t="inlineStr"/>
+      <c r="C58" t="inlineStr">
         <is>
           <t>A.7 (Physical Controls)</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
+      <c r="D58" t="inlineStr">
         <is>
           <t>A.7.12</t>
         </is>
       </c>
-      <c r="D58" t="inlineStr">
+      <c r="E58" t="inlineStr">
         <is>
           <t>Cabling security</t>
         </is>
       </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>No information on cabling security to prevent interception or damage.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Implement and document cabling security measures.</t>
+          <t>No mention of cabling security controls.</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>No controls for securing cabling infrastructure.</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>Establish and document cabling security controls.</t>
         </is>
       </c>
     </row>
@@ -2376,34 +2872,40 @@
       <c r="A59" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="B59" t="inlineStr">
+      <c r="B59" t="inlineStr"/>
+      <c r="C59" t="inlineStr">
         <is>
           <t>A.7 (Physical Controls)</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr">
+      <c r="D59" t="inlineStr">
         <is>
           <t>A.7.13</t>
         </is>
       </c>
-      <c r="D59" t="inlineStr">
+      <c r="E59" t="inlineStr">
         <is>
           <t>Equipment maintenance</t>
         </is>
       </c>
-      <c r="E59" t="inlineStr">
+      <c r="F59" t="inlineStr">
         <is>
           <t>🟡</t>
         </is>
       </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>The document mentions repair and purchasing of equipment in the restoration phase but does not detail a formal equipment maintenance process or schedule.</t>
-        </is>
-      </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Establish and document a formal equipment maintenance policy and procedures to ensure equipment is regularly maintained to prevent failures.</t>
+          <t>Section 3.2 mentions decisions about purchasing new equipment or repairing existing equipment after incidents.</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>No detailed procedures or schedules for regular equipment maintenance are described.</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>Establish and document formal equipment maintenance procedures and schedules to ensure ongoing maintenance and reliability.</t>
         </is>
       </c>
     </row>
@@ -2411,34 +2913,40 @@
       <c r="A60" s="1" t="n">
         <v>58</v>
       </c>
-      <c r="B60" t="inlineStr">
+      <c r="B60" t="inlineStr"/>
+      <c r="C60" t="inlineStr">
         <is>
           <t>A.7 (Physical Controls)</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
+      <c r="D60" t="inlineStr">
         <is>
           <t>A.7.14</t>
         </is>
       </c>
-      <c r="D60" t="inlineStr">
+      <c r="E60" t="inlineStr">
         <is>
           <t>Secure disposal or re‑use of equipment</t>
         </is>
       </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>No mention of secure disposal or re-use of equipment is found in the document.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Develop and include procedures for secure disposal or re-use of equipment to prevent unauthorized access to information.</t>
+          <t>No mention of secure disposal or reuse of equipment in the document.</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>Lack of policies or procedures for secure disposal or reuse of equipment to prevent data leakage or unauthorized access.</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>Develop and implement procedures for secure disposal and reuse of equipment, including data sanitization and environmental considerations.</t>
         </is>
       </c>
     </row>
@@ -2448,32 +2956,42 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr">
+      <c r="D61" t="inlineStr">
         <is>
           <t>A.8.1</t>
         </is>
       </c>
-      <c r="D61" t="inlineStr">
+      <c r="E61" t="inlineStr">
         <is>
           <t>User endpoint devices</t>
         </is>
       </c>
-      <c r="E61" t="inlineStr">
+      <c r="F61" t="inlineStr">
         <is>
           <t>🟡</t>
         </is>
       </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>The document references workstations and laptops in recovery plans but lacks specific controls or policies for managing user endpoint devices.</t>
-        </is>
-      </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Implement and document controls for managing user endpoint devices including configuration, security, and usage policies.</t>
+          <t>Section 2.9 lists IT and communications equipment required for recovery, including workstations and mobile phones, but no detailed controls on endpoint security.</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>No explicit mention of endpoint device security controls such as configuration, protection, or management.</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>Include detailed endpoint device management policies covering configuration, security controls, and monitoring.</t>
         </is>
       </c>
     </row>
@@ -2481,34 +2999,40 @@
       <c r="A62" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="B62" t="inlineStr">
+      <c r="B62" t="inlineStr"/>
+      <c r="C62" t="inlineStr">
         <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr">
+      <c r="D62" t="inlineStr">
         <is>
           <t>A.8.2</t>
         </is>
       </c>
-      <c r="D62" t="inlineStr">
+      <c r="E62" t="inlineStr">
         <is>
           <t>Privileged access rights</t>
         </is>
       </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>No information on management or control of privileged access rights is provided.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Establish and document procedures for granting, reviewing, and revoking privileged access rights.</t>
+          <t>No information on management or control of privileged access rights.</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>Absence of documented controls for managing privileged access rights to systems and information.</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>Implement and document procedures for granting, reviewing, and revoking privileged access rights.</t>
         </is>
       </c>
     </row>
@@ -2518,32 +3042,42 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr">
+      <c r="D63" t="inlineStr">
         <is>
           <t>A.8.3</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr">
+      <c r="E63" t="inlineStr">
         <is>
           <t>Information access restriction</t>
         </is>
       </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>The document does not address restrictions on information access.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Define and implement access control policies to restrict information access based on roles and responsibilities.</t>
+          <t>No explicit mention of access restriction controls or mechanisms in the document.</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>Lack of documented policies or technical controls restricting access to information based on business and security requirements.</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>Define and implement access control policies and mechanisms to restrict information access appropriately.</t>
         </is>
       </c>
     </row>
@@ -2551,34 +3085,40 @@
       <c r="A64" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="B64" t="inlineStr">
+      <c r="B64" t="inlineStr"/>
+      <c r="C64" t="inlineStr">
         <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr">
+      <c r="D64" t="inlineStr">
         <is>
           <t>A.8.4</t>
         </is>
       </c>
-      <c r="D64" t="inlineStr">
+      <c r="E64" t="inlineStr">
         <is>
           <t>Access to source code</t>
         </is>
       </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F64" t="inlineStr">
         <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
           <t>No mention of controls related to access to source code.</t>
         </is>
       </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>Develop and document controls to restrict and monitor access to source code.</t>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>No documented controls or procedures for managing and restricting access to source code.</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>Establish controls and procedures to manage and restrict access to source code repositories.</t>
         </is>
       </c>
     </row>
@@ -2586,34 +3126,40 @@
       <c r="A65" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="B65" t="inlineStr">
+      <c r="B65" t="inlineStr"/>
+      <c r="C65" t="inlineStr">
         <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr">
+      <c r="D65" t="inlineStr">
         <is>
           <t>A.8.5</t>
         </is>
       </c>
-      <c r="D65" t="inlineStr">
+      <c r="E65" t="inlineStr">
         <is>
           <t>Secure authentication</t>
         </is>
       </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>No details on authentication mechanisms or policies are provided.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Implement and document secure authentication methods, including multi-factor authentication where appropriate.</t>
+          <t>No details on authentication mechanisms or policies.</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>No documented secure authentication controls such as multi-factor authentication or password policies.</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>Implement and document secure authentication mechanisms and policies.</t>
         </is>
       </c>
     </row>
@@ -2623,32 +3169,42 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr">
+      <c r="D66" t="inlineStr">
         <is>
           <t>A.8.6</t>
         </is>
       </c>
-      <c r="D66" t="inlineStr">
+      <c r="E66" t="inlineStr">
         <is>
           <t>Capacity management</t>
         </is>
       </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>No information on capacity management is included.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Establish capacity management processes to ensure IT resources meet current and future business requirements.</t>
+          <t>No mention of capacity management processes or monitoring.</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>Lack of documented capacity management to ensure availability and performance of information systems.</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>Develop and implement capacity management processes and monitoring.</t>
         </is>
       </c>
     </row>
@@ -2658,32 +3214,42 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C67" t="inlineStr">
+      <c r="D67" t="inlineStr">
         <is>
           <t>A.8.7</t>
         </is>
       </c>
-      <c r="D67" t="inlineStr">
+      <c r="E67" t="inlineStr">
         <is>
           <t>Protection against malware</t>
         </is>
       </c>
-      <c r="E67" t="inlineStr">
+      <c r="F67" t="inlineStr">
         <is>
           <t>🟡</t>
         </is>
       </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>The Incident Response Plan includes handling of malware incidents but lacks proactive malware protection controls.</t>
-        </is>
-      </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Implement and document proactive malware protection measures such as antivirus software, regular updates, and user awareness.</t>
+          <t>Appendix 1 Incident Response Plan includes response to computers affected with malware by contacting IT department.</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>No proactive malware protection controls or preventive measures described.</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>Implement and document malware protection controls including prevention, detection, and response.</t>
         </is>
       </c>
     </row>
@@ -2693,32 +3259,42 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr">
+      <c r="D68" t="inlineStr">
         <is>
           <t>A.8.8</t>
         </is>
       </c>
-      <c r="D68" t="inlineStr">
+      <c r="E68" t="inlineStr">
         <is>
           <t>Management of technical vulnerabilities</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>No mention of vulnerability management processes.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>Develop and implement a vulnerability management program including regular scanning, assessment, and remediation.</t>
+          <t>No mention of vulnerability management processes or patch management.</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>Absence of documented vulnerability identification, assessment, and remediation processes.</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>Establish and document vulnerability management and patching procedures.</t>
         </is>
       </c>
     </row>
@@ -2728,32 +3304,42 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
+      <c r="D69" t="inlineStr">
         <is>
           <t>A.8.9</t>
         </is>
       </c>
-      <c r="D69" t="inlineStr">
+      <c r="E69" t="inlineStr">
         <is>
           <t>Configuration management</t>
         </is>
       </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>No details on configuration management are provided.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Establish configuration management procedures to ensure secure and consistent configuration of IT assets.</t>
+          <t>No information on configuration management of IT systems or devices.</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>No documented configuration management processes to ensure secure and consistent configurations.</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>Implement configuration management policies and procedures.</t>
         </is>
       </c>
     </row>
@@ -2763,32 +3349,42 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr">
+      <c r="D70" t="inlineStr">
         <is>
           <t>A.8.10</t>
         </is>
       </c>
-      <c r="D70" t="inlineStr">
+      <c r="E70" t="inlineStr">
         <is>
           <t>Information deletion</t>
         </is>
       </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>No information on secure information deletion is found.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Implement policies and procedures for secure deletion of information when no longer required.</t>
+          <t>No mention of secure information deletion or data sanitization.</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>Lack of procedures for secure deletion of information when no longer required.</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>Develop and implement secure information deletion policies and procedures.</t>
         </is>
       </c>
     </row>
@@ -2796,34 +3392,40 @@
       <c r="A71" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="B71" t="inlineStr">
+      <c r="B71" t="inlineStr"/>
+      <c r="C71" t="inlineStr">
         <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr">
+      <c r="D71" t="inlineStr">
         <is>
           <t>A.8.11</t>
         </is>
       </c>
-      <c r="D71" t="inlineStr">
+      <c r="E71" t="inlineStr">
         <is>
           <t>Data masking</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F71" t="inlineStr">
         <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
           <t>No mention of data masking techniques or policies.</t>
         </is>
       </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>Consider implementing data masking controls to protect sensitive information in non-production environments.</t>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>No controls for masking sensitive data to protect confidentiality.</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>Implement data masking controls where appropriate.</t>
         </is>
       </c>
     </row>
@@ -2831,34 +3433,40 @@
       <c r="A72" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="B72" t="inlineStr">
+      <c r="B72" t="inlineStr"/>
+      <c r="C72" t="inlineStr">
         <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr">
+      <c r="D72" t="inlineStr">
         <is>
           <t>A.8.12</t>
         </is>
       </c>
-      <c r="D72" t="inlineStr">
+      <c r="E72" t="inlineStr">
         <is>
           <t>Data leakage prevention</t>
         </is>
       </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>🟡</t>
-        </is>
-      </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Data leakage incidents are addressed reactively in the Incident Response Plan but no preventive controls are described.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>Implement preventive data leakage controls such as DLP tools, policies, and user training.</t>
+          <t>No mention of data leakage prevention controls or technologies.</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>No documented controls to prevent unauthorized data exfiltration.</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>Establish data leakage prevention policies and technical controls.</t>
         </is>
       </c>
     </row>
@@ -2868,26 +3476,44 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr">
+      <c r="D73" t="inlineStr">
         <is>
           <t>A.8.13</t>
         </is>
       </c>
-      <c r="D73" t="inlineStr">
+      <c r="E73" t="inlineStr">
         <is>
           <t>Information backup</t>
         </is>
       </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>✅</t>
-        </is>
-      </c>
-      <c r="F73" t="inlineStr"/>
-      <c r="G73" t="inlineStr"/>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>🟡</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Disaster Recovery Plan and recovery plans include recovery of IT infrastructure and services; backups implied but not detailed.</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>No explicit backup policies, schedules, or testing procedures described.</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>Document and implement formal backup policies, schedules, and testing.</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -2895,26 +3521,44 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr">
+      <c r="D74" t="inlineStr">
         <is>
           <t>A.8.14</t>
         </is>
       </c>
-      <c r="D74" t="inlineStr">
+      <c r="E74" t="inlineStr">
         <is>
           <t>Redundancy of information processing facilities</t>
         </is>
       </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>✅</t>
-        </is>
-      </c>
-      <c r="F74" t="inlineStr"/>
-      <c r="G74" t="inlineStr"/>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>🟡</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>Section 2.7 and 2.9 mention alternative sites and recovery time objectives implying redundancy.</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>No detailed description of redundancy mechanisms or failover procedures.</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>Document redundancy strategies and failover procedures for critical systems.</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -2922,32 +3566,42 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C75" t="inlineStr">
+      <c r="D75" t="inlineStr">
         <is>
           <t>A.8.15</t>
         </is>
       </c>
-      <c r="D75" t="inlineStr">
+      <c r="E75" t="inlineStr">
         <is>
           <t>Logging</t>
         </is>
       </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>No mention of logging or log management.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Establish logging and log management policies and procedures to record and review relevant events.</t>
+          <t>No mention of logging policies, log management, or review processes.</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>Absence of logging and monitoring controls to detect and investigate security events.</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>Implement logging policies and procedures including log review and retention.</t>
         </is>
       </c>
     </row>
@@ -2957,32 +3611,42 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C76" t="inlineStr">
+      <c r="D76" t="inlineStr">
         <is>
           <t>A.8.16</t>
         </is>
       </c>
-      <c r="D76" t="inlineStr">
+      <c r="E76" t="inlineStr">
         <is>
           <t>Monitoring activities</t>
         </is>
       </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>No information on monitoring activities is provided.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Implement monitoring controls to detect and respond to security events and anomalies.</t>
+          <t>No mention of monitoring activities or security event detection.</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>No documented monitoring controls to detect security incidents or performance issues.</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>Establish monitoring processes and tools for security and operational activities.</t>
         </is>
       </c>
     </row>
@@ -2992,32 +3656,42 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C77" t="inlineStr">
+      <c r="D77" t="inlineStr">
         <is>
           <t>A.8.17</t>
         </is>
       </c>
-      <c r="D77" t="inlineStr">
+      <c r="E77" t="inlineStr">
         <is>
           <t>Clock synchronisation</t>
         </is>
       </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>The document does not mention any policy or procedure related to clock synchronization of information systems.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Establish and document procedures to ensure accurate and consistent clock synchronization across all relevant systems to support event logging and security monitoring.</t>
+          <t>No mention of clock synchronisation or time source management in the document.</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>Lack of documented procedures or controls for clock synchronisation across systems.</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>Establish and document procedures to ensure all information systems use synchronized clocks from a reliable time source.</t>
         </is>
       </c>
     </row>
@@ -3025,34 +3699,40 @@
       <c r="A78" s="1" t="n">
         <v>76</v>
       </c>
-      <c r="B78" t="inlineStr">
+      <c r="B78" t="inlineStr"/>
+      <c r="C78" t="inlineStr">
         <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C78" t="inlineStr">
+      <c r="D78" t="inlineStr">
         <is>
           <t>A.8.18</t>
         </is>
       </c>
-      <c r="D78" t="inlineStr">
+      <c r="E78" t="inlineStr">
         <is>
           <t>Use of privileged utility programs</t>
         </is>
       </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>No reference to controls or policies governing the use of privileged utility programs is found in the document.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Develop and implement policies and controls to restrict and monitor the use of privileged utility programs to prevent unauthorized system changes or data access.</t>
+          <t>No reference to controls or management of privileged utility programs in the document.</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>No documented controls or restrictions on the use of privileged utility programs.</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>Implement and document controls governing the use of privileged utility programs to prevent unauthorized or accidental misuse.</t>
         </is>
       </c>
     </row>
@@ -3060,34 +3740,40 @@
       <c r="A79" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="B79" t="inlineStr">
+      <c r="B79" t="inlineStr"/>
+      <c r="C79" t="inlineStr">
         <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C79" t="inlineStr">
+      <c r="D79" t="inlineStr">
         <is>
           <t>A.8.19</t>
         </is>
       </c>
-      <c r="D79" t="inlineStr">
+      <c r="E79" t="inlineStr">
         <is>
           <t>Installation of software on operational systems</t>
         </is>
       </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>The document does not address controls or procedures for the installation of software on operational systems.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Define and enforce procedures for software installation on operational systems, including authorization, testing, and documentation requirements.</t>
+          <t>No mention of software installation controls or approval processes in the document.</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Absence of documented procedures for controlled installation of software on operational systems.</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>Develop and implement formal procedures for software installation, including approval, testing, and documentation.</t>
         </is>
       </c>
     </row>
@@ -3097,32 +3783,42 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C80" t="inlineStr">
+      <c r="D80" t="inlineStr">
         <is>
           <t>A.8.20</t>
         </is>
       </c>
-      <c r="D80" t="inlineStr">
+      <c r="E80" t="inlineStr">
         <is>
           <t>Network security</t>
         </is>
       </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>No explicit mention of network security controls, such as firewalls, intrusion detection, or network segmentation, is present.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Implement and document network security measures to protect the organization's information systems and data from unauthorized access and threats.</t>
+          <t>No explicit mention of network security controls or measures in the document.</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>Lack of documented network security policies, controls, or architecture.</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>Establish and document network security controls including perimeter defenses, monitoring, and access restrictions.</t>
         </is>
       </c>
     </row>
@@ -3130,34 +3826,40 @@
       <c r="A81" s="1" t="n">
         <v>79</v>
       </c>
-      <c r="B81" t="inlineStr">
+      <c r="B81" t="inlineStr"/>
+      <c r="C81" t="inlineStr">
         <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C81" t="inlineStr">
+      <c r="D81" t="inlineStr">
         <is>
           <t>A.8.21</t>
         </is>
       </c>
-      <c r="D81" t="inlineStr">
+      <c r="E81" t="inlineStr">
         <is>
           <t>Security of network services</t>
         </is>
       </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>The document lacks information on securing network services, including service configuration, monitoring, and access control.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>Establish controls to secure network services, ensuring they are configured securely, monitored, and access is restricted to authorized users.</t>
+          <t>No reference to security measures for network services in the document.</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>No documented controls ensuring security of network services.</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>Define and implement security requirements and controls for network services.</t>
         </is>
       </c>
     </row>
@@ -3165,34 +3867,40 @@
       <c r="A82" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="B82" t="inlineStr">
+      <c r="B82" t="inlineStr"/>
+      <c r="C82" t="inlineStr">
         <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C82" t="inlineStr">
+      <c r="D82" t="inlineStr">
         <is>
           <t>A.8.22</t>
         </is>
       </c>
-      <c r="D82" t="inlineStr">
+      <c r="E82" t="inlineStr">
         <is>
           <t>Segregation of networks</t>
         </is>
       </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>No details on network segregation or segmentation to separate critical systems or data are provided.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>Implement network segregation to isolate critical systems and sensitive data, reducing the risk of unauthorized access or spread of incidents.</t>
+          <t>No mention of network segregation or segmentation controls.</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>No evidence of network segregation to separate critical systems or environments.</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>Implement network segregation to isolate critical systems and reduce risk exposure.</t>
         </is>
       </c>
     </row>
@@ -3202,32 +3910,42 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C83" t="inlineStr">
+      <c r="D83" t="inlineStr">
         <is>
           <t>A.8.23</t>
         </is>
       </c>
-      <c r="D83" t="inlineStr">
+      <c r="E83" t="inlineStr">
         <is>
           <t>Web filtering</t>
         </is>
       </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>There is no mention of web filtering controls to restrict or monitor web access.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Introduce web filtering mechanisms to control and monitor internet usage, preventing access to malicious or inappropriate websites.</t>
+          <t>No mention of web filtering or controls to restrict web access.</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>Absence of web filtering controls to prevent access to malicious or inappropriate websites.</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>Implement web filtering solutions and document policies to control web access.</t>
         </is>
       </c>
     </row>
@@ -3235,34 +3953,40 @@
       <c r="A84" s="1" t="n">
         <v>82</v>
       </c>
-      <c r="B84" t="inlineStr">
+      <c r="B84" t="inlineStr"/>
+      <c r="C84" t="inlineStr">
         <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C84" t="inlineStr">
+      <c r="D84" t="inlineStr">
         <is>
           <t>A.8.24</t>
         </is>
       </c>
-      <c r="D84" t="inlineStr">
+      <c r="E84" t="inlineStr">
         <is>
           <t>Use of cryptography</t>
         </is>
       </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>The document does not reference the use of cryptographic controls for protecting information confidentiality, integrity, or authenticity.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Define and implement cryptographic controls aligned with organizational requirements and legal/regulatory obligations.</t>
+          <t>No reference to cryptographic controls or use of encryption in the document.</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>No documented cryptographic policies or controls for protecting information.</t>
+        </is>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>Develop and implement cryptographic policies and procedures aligned with business requirements.</t>
         </is>
       </c>
     </row>
@@ -3270,34 +3994,40 @@
       <c r="A85" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="B85" t="inlineStr">
+      <c r="B85" t="inlineStr"/>
+      <c r="C85" t="inlineStr">
         <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C85" t="inlineStr">
+      <c r="D85" t="inlineStr">
         <is>
           <t>A.8.25</t>
         </is>
       </c>
-      <c r="D85" t="inlineStr">
+      <c r="E85" t="inlineStr">
         <is>
           <t>Secure development life cycle</t>
         </is>
       </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>No information is provided regarding secure development lifecycle practices.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>Establish and document secure development lifecycle processes to integrate security at each phase of software development.</t>
+          <t>No mention of secure development lifecycle processes or controls.</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>Lack of documented secure development lifecycle practices.</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>Establish and document secure development lifecycle processes including security requirements, design, implementation, and testing.</t>
         </is>
       </c>
     </row>
@@ -3307,32 +4037,42 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr">
+      <c r="D86" t="inlineStr">
         <is>
           <t>A.8.26</t>
         </is>
       </c>
-      <c r="D86" t="inlineStr">
+      <c r="E86" t="inlineStr">
         <is>
           <t>Application security requirements</t>
         </is>
       </c>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>The document does not specify application security requirements or controls.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Define and enforce application security requirements to ensure applications are designed and maintained securely.</t>
+          <t>No documented application security requirements or controls found.</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>Absence of defined security requirements for applications.</t>
+        </is>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>Define and document application security requirements as part of development and procurement processes.</t>
         </is>
       </c>
     </row>
@@ -3340,34 +4080,40 @@
       <c r="A87" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="B87" t="inlineStr">
+      <c r="B87" t="inlineStr"/>
+      <c r="C87" t="inlineStr">
         <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C87" t="inlineStr">
+      <c r="D87" t="inlineStr">
         <is>
           <t>A.8.27</t>
         </is>
       </c>
-      <c r="D87" t="inlineStr">
+      <c r="E87" t="inlineStr">
         <is>
           <t>Secure systems architecture and engineering principles</t>
         </is>
       </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>No mention of secure architecture or engineering principles for systems.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>Adopt and document secure architecture and engineering principles to guide system design and implementation.</t>
+          <t>No mention of secure architecture or engineering principles in the document.</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>No evidence of secure design principles applied to systems architecture.</t>
+        </is>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>Develop and apply secure architecture and engineering principles for system design and implementation.</t>
         </is>
       </c>
     </row>
@@ -3377,32 +4123,42 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C88" t="inlineStr">
+      <c r="D88" t="inlineStr">
         <is>
           <t>A.8.28</t>
         </is>
       </c>
-      <c r="D88" t="inlineStr">
+      <c r="E88" t="inlineStr">
         <is>
           <t>Secure coding</t>
         </is>
       </c>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>There is no reference to secure coding practices or guidelines.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>Implement secure coding standards and training to reduce vulnerabilities in software development.</t>
+          <t>No reference to secure coding practices or guidelines.</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>No documented secure coding standards or training.</t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>Implement secure coding standards and provide training to developers.</t>
         </is>
       </c>
     </row>
@@ -3412,32 +4168,42 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C89" t="inlineStr">
+      <c r="D89" t="inlineStr">
         <is>
           <t>A.8.29</t>
         </is>
       </c>
-      <c r="D89" t="inlineStr">
+      <c r="E89" t="inlineStr">
         <is>
           <t>Security testing in development and acceptance</t>
         </is>
       </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>The document does not address security testing during development or acceptance phases.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>Integrate security testing into development and acceptance processes to identify and remediate vulnerabilities early.</t>
+          <t>No mention of security testing during development or acceptance phases.</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>Lack of documented security testing procedures for development and acceptance.</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>Establish security testing requirements and integrate them into development and acceptance processes.</t>
         </is>
       </c>
     </row>
@@ -3445,34 +4211,40 @@
       <c r="A90" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="B90" t="inlineStr">
+      <c r="B90" t="inlineStr"/>
+      <c r="C90" t="inlineStr">
         <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C90" t="inlineStr">
+      <c r="D90" t="inlineStr">
         <is>
           <t>A.8.30</t>
         </is>
       </c>
-      <c r="D90" t="inlineStr">
+      <c r="E90" t="inlineStr">
         <is>
           <t>Outsourced development</t>
         </is>
       </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>No controls or policies related to outsourced development are mentioned.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>Establish controls to manage security risks associated with outsourced development, including contracts and monitoring.</t>
+          <t>No reference to controls or management of outsourced development.</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>No documented controls for managing outsourced development activities.</t>
+        </is>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>Define and implement controls for outsourced development including security requirements and monitoring.</t>
         </is>
       </c>
     </row>
@@ -3482,32 +4254,42 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C91" t="inlineStr">
+      <c r="D91" t="inlineStr">
         <is>
           <t>A.8.31</t>
         </is>
       </c>
-      <c r="D91" t="inlineStr">
+      <c r="E91" t="inlineStr">
         <is>
           <t>Separation of development, test and production environments</t>
         </is>
       </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>The document does not mention separation of development, test, and production environments.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>Implement and document segregation of development, test, and production environments to prevent unauthorized access and changes.</t>
+          <t>No mention of separation between development, test, and production environments.</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>No documented segregation of environments to prevent unauthorized access or changes.</t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>Implement and document separation of development, test, and production environments.</t>
         </is>
       </c>
     </row>
@@ -3517,32 +4299,42 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C92" t="inlineStr">
+      <c r="D92" t="inlineStr">
         <is>
           <t>A.8.32</t>
         </is>
       </c>
-      <c r="D92" t="inlineStr">
+      <c r="E92" t="inlineStr">
         <is>
           <t>Change management</t>
         </is>
       </c>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>🟡</t>
-        </is>
-      </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>The document references decision-making and authorizations related to recovery plans and purchasing during incidents but lacks explicit mention of formal change management processes for IT systems.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>Develop and formalize a comprehensive change management process covering all IT system changes, including documentation, approval, testing, and communication.</t>
+          <t>No documented change management process or controls found in the document.</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>Absence of formal change management procedures.</t>
+        </is>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>Establish and document a formal change management process including approval, testing, and communication.</t>
         </is>
       </c>
     </row>
@@ -3550,34 +4342,40 @@
       <c r="A93" s="1" t="n">
         <v>91</v>
       </c>
-      <c r="B93" t="inlineStr">
+      <c r="B93" t="inlineStr"/>
+      <c r="C93" t="inlineStr">
         <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C93" t="inlineStr">
+      <c r="D93" t="inlineStr">
         <is>
           <t>A.8.33</t>
         </is>
       </c>
-      <c r="D93" t="inlineStr">
+      <c r="E93" t="inlineStr">
         <is>
           <t>Test information</t>
         </is>
       </c>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>No information on management or protection of test information is provided.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>Establish controls to protect test information, ensuring it is handled securely and does not compromise production data or systems.</t>
+          <t>No mention of controls or handling of test information.</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>No documented procedures for protecting or managing test information.</t>
+        </is>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>Define and implement controls for the protection and management of test information.</t>
         </is>
       </c>
     </row>
@@ -3585,34 +4383,40 @@
       <c r="A94" s="1" t="n">
         <v>92</v>
       </c>
-      <c r="B94" t="inlineStr">
+      <c r="B94" t="inlineStr"/>
+      <c r="C94" t="inlineStr">
         <is>
           <t>A.8 (Technological Controls)</t>
         </is>
       </c>
-      <c r="C94" t="inlineStr">
+      <c r="D94" t="inlineStr">
         <is>
           <t>A.8.34</t>
         </is>
       </c>
-      <c r="D94" t="inlineStr">
+      <c r="E94" t="inlineStr">
         <is>
           <t>Protection of information systems during audit testing</t>
         </is>
       </c>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t>❌</t>
-        </is>
-      </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>The document does not address protection of information systems during audit testing.</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>Define and implement controls to protect information systems during audit testing to prevent disruption or unauthorized access.</t>
+          <t>No reference to protection of information systems during audit testing.</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>No documented controls to protect systems during audit testing activities.</t>
+        </is>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>Establish procedures to ensure information systems are protected during audit testing.</t>
         </is>
       </c>
     </row>

</xml_diff>